<commit_message>
fixed a few bugs in co-occurrence feature gathering
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -75,7 +75,7 @@
     <t>ACLrd</t>
   </si>
   <si>
-    <t>304,205 cterms</t>
+    <t>cutoff=2</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -517,7 +517,7 @@
     <col min="1" max="1" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,11 +533,14 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1">
+        <v>148039</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -551,13 +554,13 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="H2" s="1">
-        <v>2.5694444444444447E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3.2638888888888891E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -570,8 +573,14 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.5131944444444445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -585,13 +594,13 @@
         <v>15</v>
       </c>
       <c r="G4">
-        <v>5.9</v>
+        <v>5.98</v>
       </c>
       <c r="H4" s="1">
-        <v>0.66180555555555554</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.74444444444444446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -604,8 +613,14 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>2.72</v>
+      </c>
+      <c r="H5" s="1">
+        <v>8.1944444444444445E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -619,7 +634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -633,7 +648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -647,7 +662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -661,7 +676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -675,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -689,7 +704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
added functionality to filter POS pattern extracted candidates by, e.g., min/max chars, leading stopwords etc
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -509,7 +509,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +647,12 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
+      <c r="G7">
+        <v>1.67</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3.3333333333333333E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -661,6 +667,12 @@
       <c r="F8" t="s">
         <v>11</v>
       </c>
+      <c r="G8">
+        <v>6.3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8.9583333333333334E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -675,6 +687,12 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
+      <c r="G9">
+        <v>1.45</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.4999999999999998E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -689,6 +707,12 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
+      <c r="G10">
+        <v>1.45</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2.1527777777777781E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -703,6 +727,12 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
+      <c r="G11">
+        <v>2.44</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3.7499999999999999E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -716,6 +746,12 @@
       </c>
       <c r="F12" t="s">
         <v>16</v>
+      </c>
+      <c r="G12">
+        <v>16.5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.4756944444444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>